<commit_message>
base de datos poblada
</commit_message>
<xml_diff>
--- a/Cálculo_precio_total.xlsx
+++ b/Cálculo_precio_total.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdb0fad47d4c68db/Documentos/Programación/Full Stack/13. Bases de datos SQL/Prueba 03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0BA0149-69BA-BA41-837B-0CDF50CB2A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{A0BA0149-69BA-BA41-837B-0CDF50CB2A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B8A0104-EE11-834C-ADC5-764A1ED7309D}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{15ABBEF7-D431-624E-B6AF-4A14A98A52A9}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1ABD8A-B70B-CE4F-A5A6-080BA7332EA3}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,6 +472,182 @@
         <v>210000</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:F8" si="0">(D4-1)*10000</f>
+        <v>20000</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F11" si="1">C4*E4</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9" si="2">(D9-1)*10000</f>
+        <v>60000</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10" si="3">(D10-1)*10000</f>
+        <v>10000</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11" si="4">(D11-1)*10000</f>
+        <v>30000</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>